<commit_message>
Privacy test excel file update
</commit_message>
<xml_diff>
--- a/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/MIRA_Websites_Germany.xlsx
+++ b/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/MIRA_Websites_Germany.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28680" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="17670" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="2018-01-12_DocumentList_Website" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="233">
   <si>
     <t>Domain</t>
   </si>
@@ -710,6 +711,9 @@
   </si>
   <si>
     <t>NexvarGermany</t>
+  </si>
+  <si>
+    <t>Privacy Found (Y/N)</t>
   </si>
 </sst>
 </file>
@@ -1206,51 +1210,79 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1260,9 +1292,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1300,7 +1332,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1372,7 +1404,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1546,20 +1578,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1569,8 +1602,11 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1581,7 +1617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1592,7 +1628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1603,7 +1639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1614,7 +1650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1625,7 +1661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1647,7 +1683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1658,7 +1694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1669,7 +1705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1680,7 +1716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -1691,7 +1727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -1702,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -1713,7 +1749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1724,7 +1760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
GDPR privacy data update
</commit_message>
<xml_diff>
--- a/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/MIRA_Websites_Germany.xlsx
+++ b/Bayer-Automation/src/test/java/com/bayer/corp/Regions/Germany/GDPR/config/MIRA_Websites_Germany.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="2018-01-12_DocumentList_Website" sheetId="1" r:id="rId1"/>
+    <sheet name="URL Output" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="262">
   <si>
     <t>Domain</t>
   </si>
@@ -713,14 +713,101 @@
     <t>NexvarGermany</t>
   </si>
   <si>
-    <t>Privacy Found (Y/N)</t>
+    <t>https://www.pallas-versicherung.de</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Prviacy Found(T/F)</t>
+  </si>
+  <si>
+    <t>Privacy Name</t>
+  </si>
+  <si>
+    <t>Phrase 1 Found</t>
+  </si>
+  <si>
+    <t>Phrase 2 Found</t>
+  </si>
+  <si>
+    <t>Phrase 3 Found</t>
+  </si>
+  <si>
+    <t>Phrase 4 Found</t>
+  </si>
+  <si>
+    <t>Phrase 5 Found</t>
+  </si>
+  <si>
+    <t>https://www.cropscience.bayer.de</t>
+  </si>
+  <si>
+    <t>Datenschutzerklärung</t>
+  </si>
+  <si>
+    <t>http://www.aktren.de/index.html</t>
+  </si>
+  <si>
+    <t>https://www.aspirin.de/</t>
+  </si>
+  <si>
+    <t>https://www.lefax.de/</t>
+  </si>
+  <si>
+    <t>https://xofigo.de/de</t>
+  </si>
+  <si>
+    <t>http://darmstadt.bayer.de/</t>
+  </si>
+  <si>
+    <t>https://www.seresto.de/</t>
+  </si>
+  <si>
+    <t>https://www.lungenhochdruck.de</t>
+  </si>
+  <si>
+    <t>https://www.baylab.bayer.de/</t>
+  </si>
+  <si>
+    <t>http://pharma.bayer.com/</t>
+  </si>
+  <si>
+    <t>Policy name not found</t>
+  </si>
+  <si>
+    <t>http://www.digital-farming.de/</t>
+  </si>
+  <si>
+    <t>https://leganto.bayer.de/</t>
+  </si>
+  <si>
+    <t>https://legaplus.bayer.de</t>
+  </si>
+  <si>
+    <t>http://www.nunhems.de/</t>
+  </si>
+  <si>
+    <t>http://www.clipmyfarm.de/</t>
+  </si>
+  <si>
+    <t>https://www.premeo.de/</t>
+  </si>
+  <si>
+    <t>http://pim.bayergarten.de/Default.aspx</t>
+  </si>
+  <si>
+    <t>https://www.environmentalscience.bayer.de/</t>
+  </si>
+  <si>
+    <t>http://agrar.bayer.de/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,8 +926,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1020,6 +1121,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1152,7 +1259,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1195,8 +1302,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1208,8 +1316,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1243,6 +1358,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1578,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1592,7 +1708,7 @@
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1602,172 +1718,169 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1775,10 +1888,10 @@
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1786,10 +1899,10 @@
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1797,10 +1910,10 @@
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1808,10 +1921,10 @@
       <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2165,7 +2278,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>105</v>
       </c>
@@ -2462,7 +2575,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>158</v>
       </c>
@@ -2616,7 +2729,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="94" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>185</v>
       </c>
@@ -2879,6 +2992,555 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
+    <col min="5" max="5" width="18.25" customWidth="1"/>
+    <col min="6" max="6" width="16.25" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>252</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>242</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>252</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>261</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>242</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>